<commit_message>
Updated the TA472 sheet and modified the method names of wish list classes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA472.xlsx
+++ b/src/test/resources/data/jdgroupTA472.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ADF349-2BAA-4446-B524-E9A4B5DA40D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D756CB7D-37F8-4463-89A9-854D5D359235}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26572,10 +26572,10 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -26962,7 +26962,7 @@
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="111" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="57" t="s">
         <v>859</v>
@@ -27113,7 +27113,7 @@
       </c>
       <c r="E16" s="56"/>
       <c r="F16" s="111" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G16" s="116" t="s">
         <v>859</v>

</xml_diff>